<commit_message>
added a script to generate a Hadoop configuration in Coq's format
</commit_message>
<xml_diff>
--- a/bin/Hadoop_params_real_world_type.xlsx
+++ b/bin/Hadoop_params_real_world_type.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="changeable" sheetId="1" state="visible" r:id="rId2"/>
@@ -1403,7 +1403,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1433,12 +1433,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1489,7 +1483,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1510,10 +1504,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1526,7 +1516,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1550,24 +1540,25 @@
   <dimension ref="A1:AC107"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C106" activeCellId="0" sqref="C106:C107"/>
+      <selection pane="bottomLeft" activeCell="C96" activeCellId="0" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.1530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.6020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.8979591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.6377551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.8265306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="10" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="29" min="20" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.5408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.3571428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.8265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="19" min="10" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="29" min="20" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,7 +1615,7 @@
       <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1666,7 +1657,7 @@
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="5" t="n">
         <v>128</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1711,7 +1702,7 @@
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1756,7 +1747,7 @@
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="5" t="n">
         <v>1000000</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1801,7 +1792,7 @@
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="5" t="n">
         <v>1000000</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1848,10 +1839,10 @@
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="6" t="n">
         <v>67108864</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1954,7 +1945,7 @@
       <c r="G9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="8" t="s">
         <v>46</v>
       </c>
       <c r="I9" s="3"/>
@@ -2089,7 +2080,7 @@
       <c r="G12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>62</v>
       </c>
       <c r="I12" s="3"/>
@@ -2224,7 +2215,7 @@
       <c r="G15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="8" t="s">
         <v>76</v>
       </c>
       <c r="I15" s="3"/>
@@ -3825,7 +3816,7 @@
       <c r="B51" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="4" t="s">
         <v>213</v>
       </c>
       <c r="D51" s="4" t="s">
@@ -5262,10 +5253,10 @@
       <c r="A83" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="B83" s="7" t="n">
+      <c r="B83" s="6" t="n">
         <v>20480</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="5" t="s">
         <v>332</v>
       </c>
       <c r="D83" s="4" t="s">
@@ -5843,7 +5834,7 @@
       <c r="AB95" s="3"/>
       <c r="AC95" s="3"/>
     </row>
-    <row r="96" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
         <v>369</v>
       </c>
@@ -6027,10 +6018,10 @@
       <c r="A100" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="B100" s="7" t="n">
+      <c r="B100" s="6" t="n">
         <v>2048</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="C100" s="5" t="s">
         <v>388</v>
       </c>
       <c r="D100" s="4" t="s">
@@ -6252,7 +6243,7 @@
       <c r="A105" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="B105" s="7" t="n">
+      <c r="B105" s="6" t="n">
         <v>3600</v>
       </c>
       <c r="C105" s="4" t="s">

</xml_diff>

<commit_message>
fixed field sequence in all files
</commit_message>
<xml_diff>
--- a/bin/Hadoop_params_real_world_type.xlsx
+++ b/bin/Hadoop_params_real_world_type.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">65536</t>
   </si>
   <si>
-    <t xml:space="preserve">52428, 58982, 72090, 78644</t>
+    <t xml:space="preserve">57344, 61440, 69632, 73728</t>
   </si>
   <si>
     <t xml:space="preserve">nature number</t>
@@ -1540,25 +1540,25 @@
   <dimension ref="A1:AC107"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C96" activeCellId="0" sqref="C96"/>
+      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.5408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.3571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.8265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="19" min="10" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="29" min="20" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.1530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="10" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="29" min="20" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,7 +1608,7 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>